<commit_message>
HouseKeeping, Commenting and Minor modify Done
</commit_message>
<xml_diff>
--- a/Database Structure.xlsx
+++ b/Database Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13800" windowHeight="10575"/>
+    <workbookView windowWidth="27720" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Table name</t>
   </si>
@@ -103,6 +103,12 @@
     <t>answer</t>
   </si>
   <si>
+    <t>vote</t>
+  </si>
+  <si>
+    <t>default = 0</t>
+  </si>
+  <si>
     <t>question_id</t>
   </si>
   <si>
@@ -116,15 +122,6 @@
   </si>
   <si>
     <t>Answer (id)</t>
-  </si>
-  <si>
-    <t>isVoted</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>default = false</t>
   </si>
 </sst>
 </file>
@@ -132,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -146,24 +143,93 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,7 +244,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,101 +280,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -299,187 +296,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,30 +506,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -547,11 +520,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,8 +549,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,153 +578,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1066,7 +1063,7 @@
   <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -1257,9 +1254,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:8">
       <c r="C16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1267,16 +1264,13 @@
       <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="F16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
+      <c r="H16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1288,32 +1282,32 @@
         <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7">
-      <c r="C20" t="s">
-        <v>32</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -1325,21 +1319,24 @@
         <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
       <c r="C21" t="s">
         <v>34</v>
       </c>
       <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
         <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>